<commit_message>
Replace gantt_chart.xlsx with this weeks updated version
</commit_message>
<xml_diff>
--- a/Planning/gantt_chart.xlsx
+++ b/Planning/gantt_chart.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adven\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\bodiam\ATT\aj418\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C28C40BF-ABE5-460F-BA70-EEA15755D799}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Task</t>
   </si>
@@ -91,12 +90,18 @@
   </si>
   <si>
     <t>jj</t>
+  </si>
+  <si>
+    <t>Login Implementation</t>
+  </si>
+  <si>
+    <t>Alice and Kieran</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -198,9 +203,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Start Date</c:v>
-          </c:tx>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -211,9 +213,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Testing Plan</c:v>
                 </c:pt>
@@ -234,16 +236,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Class Diagram</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Login Implementation</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:f>Sheet1!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>43494</c:v>
                 </c:pt>
@@ -264,6 +269,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>43497</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -277,9 +285,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Duration</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -292,9 +297,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Testing Plan</c:v>
                 </c:pt>
@@ -315,16 +320,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Class Diagram</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Login Implementation</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:f>Sheet1!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -340,11 +348,8 @@
                 <c:pt idx="4">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -487,6 +492,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -494,7 +500,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1377,11 +1382,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1439,7 +1444,7 @@
         <v>43494</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D6" si="0">E3-C3</f>
+        <f t="shared" ref="D3:D8" si="0">E3-C3</f>
         <v>2</v>
       </c>
       <c r="E3" s="1">
@@ -1510,9 +1515,6 @@
       <c r="C7" s="1">
         <v>43497</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
       <c r="E7" t="s">
         <v>18</v>
       </c>
@@ -1528,13 +1530,26 @@
         <v>43497</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>43504</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1">
+        <v>43501</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
       <c r="M9" t="s">
         <v>19</v>
       </c>

</xml_diff>